<commit_message>
service adjustment, uat feedback
</commit_message>
<xml_diff>
--- a/assets/format/template_export_stock_take.xlsx
+++ b/assets/format/template_export_stock_take.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\sgss-web\assets\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B99643-212C-4B21-926A-8357B1928D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5748CAC5-9BF3-45B0-A7E4-C22A50DFF1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2F15F523-A8F8-4B01-A65B-6B4F5ED804C2}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,11 +484,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{361FDA0A-AA78-46CC-BB6F-B23E9C998599}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>